<commit_message>
change intro, some analysis fixes
</commit_message>
<xml_diff>
--- a/graph/ss.xlsx
+++ b/graph/ss.xlsx
@@ -12,57 +12,138 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="118">
   <si>
     <t>Text</t>
   </si>
   <si>
-    <t>BIS_19, ИУ7-53Б, Авдейкина Валерия 1InСОДЕРЖАНИЕ ВВЕДЕНИЕ 3 1 Обзор вейвлет-шума 4 1.1 Алгоритм .</t>
+    <t>Министерство науки и высшего образования Российской Федерации Федеральное государственное бюджетное образовательное учреждение высшего образования «Московский государственный технический университет имени Н.</t>
+  </si>
+  <si>
+    <t>Э.</t>
+  </si>
+  <si>
+    <t>Баумана (национальный исследовательский университет)» (МГТУ им.</t>
+  </si>
+  <si>
+    <t>Н.</t>
+  </si>
+  <si>
+    <t>Баумана) ФАКУЛЬТЕТ «Информатика исистемы управления» КАФЕДРА «Программное обеспечение ЭВМ иинформационные технологии» РАСЧЕТНО-ПОЯСНИТЕЛЬНАЯ ЗАПИСКА К НАУЧНО-ИССЛЕДОВАТЕЛЬСКОЙ РАБОТЕ НА ТЕМУ: «Вейвлет-шум» Студент ИУ7-53Б(BIS_19) (Группа) (Подпись, дата)Авдейкина В.</t>
+  </si>
+  <si>
+    <t>П.</t>
+  </si>
+  <si>
+    <t>(И.</t>
+  </si>
+  <si>
+    <t>О.</t>
+  </si>
+  <si>
+    <t>Фамилия) Руководитель НИР (Подпись, дата)Кострицкий А.</t>
+  </si>
+  <si>
+    <t>С.</t>
+  </si>
+  <si>
+    <t>Фамилия) 2023 г.InСОДЕРЖАНИЕ ВВЕДЕНИЕ 3 1 Обзор вейвлет-шума 4 1.1 Математические основы .</t>
   </si>
   <si>
     <t>.</t>
   </si>
   <si>
-    <t>4 1.1.1 Получение из R↓.</t>
-  </si>
-  <si>
-    <t>4 1.1.2 Получение R↓↑.</t>
-  </si>
-  <si>
-    <t>5 1.1.3 Получение N.</t>
-  </si>
-  <si>
-    <t>5 СПИСОК ИСПОЛЬЗОВАННЫХ ИСТОЧНИКОВ 7 2InВВЕДЕНИЕ За последние 15 лет генерация поверхностей не перестала быть актуальной задачей компьютерной графики и упоминается в [1—5].</t>
-  </si>
-  <si>
-    <t>Таким образом, возникает необходимость нахождения методов, которые позволят облегчить решение этой задачи.</t>
-  </si>
-  <si>
-    <t>Существует ряд методов, суть которых заключается в использовании шумов – генераторов последовательностей случайных чисел [6].</t>
-  </si>
-  <si>
-    <t>Одним из таких методов является метод вейвлет-шума (вейвлет-шум) [7; 8], который будет рассмотрен далее.</t>
-  </si>
-  <si>
-    <t>3In1 Обзор вейвлет-шума Вейвлет-шум основывается на вейвлет-функциях – функциях независимой переменной, имеющих вид коротких волн, которые можно сдвигать и масштабировать вдоль оси независимой переменной с помощью соответствующих параметров [9—11].</t>
-  </si>
-  <si>
-    <t>Пример вейвлета можно наблюдать на рис.</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>[рисунок 1 – пример графика вейвлет функции] Множество вейвлетов, которые могут быть получены с помощью линейной комбинации некоторых функций, называется семейством вейвлетов, а эти функции – базисными функциями семейства.</t>
-  </si>
-  <si>
-    <t>[9—12] Входными данными метода: изображение R.</t>
-  </si>
-  <si>
-    <t>Выходными данными метода: изображение N.</t>
-  </si>
-  <si>
-    <t>Авторы [7] представляют алгоритм вейвлет-шума тремя семантическими шагами: 1) получение R↓; 2) получение R↓↑; 3) получение N.</t>
+    <t>4 1.2 Вейвлет-шум .</t>
+  </si>
+  <si>
+    <t>5 1.2.1 Получение R↓.</t>
+  </si>
+  <si>
+    <t>6 1.2.2 Получение R↓.</t>
+  </si>
+  <si>
+    <t>6 1.2.3 Получение R↓↑.</t>
+  </si>
+  <si>
+    <t>7 1.2.4 Получение N.</t>
+  </si>
+  <si>
+    <t>7 СПИСОК ИСПОЛЬЗОВАННЫХ ИСТОЧНИКОВ 9 2InВВЕДЕНИЕ За последние 15 лет генерация поверхностей с текстурами (стилями заполнения, имитирующими сложную рельефную объемную плоскость, выполненную из какого-то материала [1]) не перестала быть актуальной задачей компьютерной графики и упоминается в [2—6].</t>
+  </si>
+  <si>
+    <t>Таким образом, возникает необходимость нахождения методов, которые обеспечивают решение этой задачи.</t>
+  </si>
+  <si>
+    <t>Существует ряд решений описанной задачи, одним из которых является использование метода вейвлет-шума (вейвлет-шум) [7; 8], который будет рассмотрен далее.</t>
+  </si>
+  <si>
+    <t>3In1 Обзор вейвлет-шума В данном разделе будут рассмотрены математические основы вейвлетшума и его описание.</t>
+  </si>
+  <si>
+    <t>1.1 Математические основы Суть вейвлет-шума заключается в использовании вейвлетов.</t>
+  </si>
+  <si>
+    <t>Вейвлет — функция независимой переменной, имеющая вид короткой волны (всплеска) [9—11].</t>
+  </si>
+  <si>
+    <t>Пример вейвлета можно наблюдать на рисунке 1.</t>
+  </si>
+  <si>
+    <t>[рисунок 1 — пример графика вейвлет функции] Центр вейвлета — значение независимой переменной, через которое проходит вертикальная ось симметрии вейвлета.</t>
+  </si>
+  <si>
+    <t>Пространство вейвлетов W— набор функций, которые могут быть представлены линейной комбинацией сдвигов и масштабирования одного вейвлета.</t>
+  </si>
+  <si>
+    <t>[12; 13] Масштабирующая функция ξ— функция, для которой справедливо следующее равенство: ξ(x) =X kpkξ(2x−k), (1.1) при условии, что существуют такие числовые коэффициенты pk.</t>
+  </si>
+  <si>
+    <t>[7; 12] Согласно [7], если ϕ(x)— функция из W, центр которой x= 0, то любая функция F(x)может быть представлена следующим образом: F(x) =X ifiϕ(x−i), (1.2) гдеϕ(x−i)— функция из Wс центром x=i,fi— некоторые числовые коэффициенты.</t>
+  </si>
+  <si>
+    <t>Пространство S0— пространство, состоящее из функций вида 1.2.</t>
+  </si>
+  <si>
+    <t>Функции G(x)вида G(x) =X igiϕ(2x−i) (1.3) аналогично составляют пространство S1.</t>
+  </si>
+  <si>
+    <t>[7] 4InЕсли рассматриваемая в 1.3, 1.2 функция ϕявляется масштабирующей, тоS1расширяет S0, то есть включает все функции S0.</t>
+  </si>
+  <si>
+    <t>[7; 12] Вейвлет-анализ — процесс определения того, расширяет ли пространство S1пространство S0.</t>
+  </si>
+  <si>
+    <t>[7].</t>
+  </si>
+  <si>
+    <t>Тогда функция F(x)из 1.2 представляется с помощью коэффициентов f↑ iв пространстве S1: F(x) =X if↑ iϕ(2x−i) (1.4) Коэффициенты f↑ iвыражаются с использованием формулы 1.1: f↑ i=X kpi−2kfk (1.5) Согласно [7], коэффициенты g↓ i, необходимые для представления функцииG(x)из 1.3 в пространстве S0, вычисляются с помощью вейвлет-анализа и являются равными g↓ i=X kak−2igk (1.6) а функция G(x)представляется как G(x) =G↓(x) +D(x) (1.7) гдеD(x)— функция из S1, которая не может быть выражена в S0через какие-либо коэффициенты.</t>
+  </si>
+  <si>
+    <t>1.2 Вейвлет-шум Изображение Xпредставляется набором числовых коэффициентов (.</t>
+  </si>
+  <si>
+    <t>, x i, .</t>
+  </si>
+  <si>
+    <t>): X= (.</t>
+  </si>
+  <si>
+    <t>) (1.8) Входные данные вейвлет-шума: функция B(x)изW, изображение R.</t>
+  </si>
+  <si>
+    <t>Выходные данные вейвлет-шума: изображение N.</t>
+  </si>
+  <si>
+    <t>Авторы [7] представляют алгоритм вейвлет-шума тремя семантическими 5Inшагами: 1) получение R(x); 2) получение R↓(x); 3) получение R↓↑(x); 4) получение N(x).</t>
+  </si>
+  <si>
+    <t>После выполнения алгоритма для получения результата значение функцииN(x)вычисляется при заданном При заданном вычисляется значение функции N(x)и получается изображение N= (.</t>
+  </si>
+  <si>
+    <t>, n i, .</t>
+  </si>
+  <si>
+    <t>).</t>
   </si>
   <si>
     <t>Пример визуализации получения результата алгоритма можно наблюдать на рис.</t>
@@ -71,13 +152,40 @@
     <t>2.</t>
   </si>
   <si>
-    <t>[рисунок 2 – пример визуализации получения из R N] В [7] авторы вводят следующие операции: повышение разрешения изображения, повышение разрешения изображения, вычитание изображений.</t>
-  </si>
-  <si>
-    <t>Если изображение Xпредставляетсяспомощьюпоследовательности X= (..., x i, ...), гдеxi– число, то упомянутые операции можно представить как ...</t>
-  </si>
-  <si>
-    <t>[описание операций] 1.1 Алгоритм Рассмотрим представленные ранее шаги более подробно 1.1.1 Получение из R↓ Пусть Rпредставлено формулой: 4In[R через свои коэф-ты ] (1.1) Используя операцию понижения разрешения и используя формулу 1.1: [R↓, r↓,коэффициенты из R ] (1.2) 1.1.2 Получение R↓↑ Применяя операцию повышения разрешения и используя формулу 1.2: [R↓↑, r↓↑,коэффициенты из R ] (1.3) 1.1.3 Получение N Применяя операцию вычитания и используя формулу 1.3: [N, n,коэффициенты из r ] (1.4) 5InСПИСОК ИСПОЛЬЗОВАННЫХ ИСТОЧНИКОВ 1.Pai H.</t>
+    <t>[рисунок 2 — пример визуализации получения из R N[7]] Рассмотрим представленные шаги более подробно, основываясь на информации из [7].</t>
+  </si>
+  <si>
+    <t>1.2.1 Получение R↓ Согласно формуле 1.8 изображение Rпредставляется следующим образом: R= (.</t>
+  </si>
+  <si>
+    <t>, r i, .</t>
+  </si>
+  <si>
+    <t>) (1.9) Аналогично формуле 1.3 выражается R(x): R=X iriB(2x−i) (1.10) 1.2.2 Получение R↓ Согласно формуле 1.7: R(x) =R↓(x) +N(x) (1.11) N(x)выражается из формулы 1.11 как N(x) =R(x)−R↓(x) (1.12) 6InС помощью формулы 1.2 получаем R↓(x) =X ir↓ iB(x−i) (1.13) гдеr↓ iвыражаются с помощью формулы 1.6: r↓ i=X kak−2irk (1.14) 1.2.3 Получение R↓↑ C помощью формул 1.10 и 1.13 выражение 1.12 преобразовывается как N(x) =X iriB(2x−i)−X ir↓ iB(x−i) (1.15) С учетом формулы 1.4 и 1.13 получается выражение R↓↑(x) =X ir↓↑ iB(2x−i) (1.16) где коэффициенты r↓↑ iвыражаются с учетом формулы 1.5: r↓↑ i=X kpi−2kr↓ k (1.17) 1.2.4 Получение N С использованием формулы 1.16 выражение 1.15 записывается как N(x) =X iriB(2x−i)−X ir↓↑ iB(2x−i) =X in′ iB(2x−i)(1.18) гдеn′ i=ri−r↓↑ i.</t>
+  </si>
+  <si>
+    <t>Для получения изображения N= (.</t>
+  </si>
+  <si>
+    <t>)значение функции N(x) вычисляется при задаваемых значениях x.</t>
+  </si>
+  <si>
+    <t>7InСПИСОК ИСПОЛЬЗОВАННЫХ ИСТОЧНИКОВ 1.Порев В.</t>
+  </si>
+  <si>
+    <t>Компьютерная графика.</t>
+  </si>
+  <si>
+    <t>— СПб : БХВ-Петербург, 2002.</t>
+  </si>
+  <si>
+    <t>— С.</t>
+  </si>
+  <si>
+    <t>432.</t>
+  </si>
+  <si>
+    <t>2.Pai H.</t>
   </si>
   <si>
     <t>-Y.Texture designs and workflows for physically based rendering using procedural texture generation //2019 IEEE Eurasia Conference on IOT, Communication and Engineering (ECICE).</t>
@@ -86,13 +194,10 @@
     <t>— 2019.</t>
   </si>
   <si>
-    <t>— С.</t>
-  </si>
-  <si>
     <t>195—198.</t>
   </si>
   <si>
-    <t>2.Weakly-Supervised Photo-realistic Texture Generation for 3D Face Reconstruction / X.</t>
+    <t>3.Weakly-Supervised Photo-realistic Texture Generation for 3D Face Reconstruction / X.</t>
   </si>
   <si>
     <t>Yin [и др.] //2023 IEEE 17th International Conference on Automatic Face and Gesture Recognition (FG).</t>
@@ -104,7 +209,7 @@
     <t>1—8.</t>
   </si>
   <si>
-    <t>3.Digital preservation of Brazilian indigenous artworks: Generating high quality textures for 3D models [Электронный ресурс] / B.</t>
+    <t>4.Digital preservation of Brazilian indigenous artworks: Generating high quality textures for 3D models [Электронный ресурс] / B.</t>
   </si>
   <si>
     <t>Trinch˜ ao Andrade [и др.] // Journal of Cultural Heritage.</t>
@@ -128,7 +233,7 @@
     <t>— URL: https: //www.sciencedirect.com/science/article/pii/S1296207411000513 (дата обращения: 24.11.2023).</t>
   </si>
   <si>
-    <t>4.Quintana G.</t>
+    <t>5.Quintana G.</t>
   </si>
   <si>
     <t>,Ciurana J.</t>
@@ -152,7 +257,7 @@
     <t>— (дата обращения: 24.11.2023).</t>
   </si>
   <si>
-    <t>5.A Papier-Mˆ ach´ e Approach to Learning 3D Surface Generation / T.</t>
+    <t>6.A Papier-Mˆ ach´ e Approach to Learning 3D Surface Generation / T.</t>
   </si>
   <si>
     <t>Groueix [и др.]//Proceedings of the IEEE Conference on Computer Vision and Pattern Recognition (CVPR).</t>
@@ -161,12 +266,6 @@
     <t>— 2018.</t>
   </si>
   <si>
-    <t>6.A Survey of Procedural Noise Functions [Электронный ресурс].</t>
-  </si>
-  <si>
-    <t>— URL: https://doi.org/10.1111/j.1467-8659.2010.01827.x (дата обращения: 11.11.2023).</t>
-  </si>
-  <si>
     <t>7.Cook R.,De Rose T.</t>
   </si>
   <si>
@@ -188,13 +287,13 @@
     <t>edu / cs448x / old / Procedural _ Noise(2f ) Categories.html (дата обращения: 11.11.2023).</t>
   </si>
   <si>
-    <t>6In9.Крыжевич Л.</t>
+    <t>9.Крыжевич Л.</t>
   </si>
   <si>
     <t>,Ковалев В.</t>
   </si>
   <si>
-    <t>Задача очистки изображения от шума и вейвлет-подходы к ее решению //Актуальные исследования в области математики, информатики, физики и методики их изучения в современном образовательном пространстве.</t>
+    <t>Задача очистки изображения от шума и вейвлет-подходы к ее решению //Актуальные исследования в области математики, информатики, физики и методики их изучения в совре8Inменном образовательном пространстве.</t>
   </si>
   <si>
     <t>— 2016.</t>
@@ -233,7 +332,28 @@
     <t>671.</t>
   </si>
   <si>
-    <t>12.Meyer Y.</t>
+    <t>12.Новиков Л.</t>
+  </si>
+  <si>
+    <t>Модифицированные вейвлеты в обработке данных аналитических приборов.</t>
+  </si>
+  <si>
+    <t>I.</t>
+  </si>
+  <si>
+    <t>основы теории.</t>
+  </si>
+  <si>
+    <t>— 2006.</t>
+  </si>
+  <si>
+    <t>— URL: https : / / cyberleninka .</t>
+  </si>
+  <si>
+    <t>ru / article / n / modifitsirovannye - veyvlety - v obrabotke-dannyh-analiticheskih-priborov-i-osnovy-teorii (дата обращения: 25.11.2023).</t>
+  </si>
+  <si>
+    <t>13.Meyer Y.</t>
   </si>
   <si>
     <t>Wavelets: Algorithms and applications.</t>
@@ -245,7 +365,7 @@
     <t>129.</t>
   </si>
   <si>
-    <t>7In.</t>
+    <t>9In.</t>
   </si>
 </sst>
 </file>
@@ -916,7 +1036,327 @@
       <c r="A78" t="s">
         <v>77</v>
       </c>
-      <c r="B78"/>
+      <c r="B78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+      <c r="B118"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>